<commit_message>
after Re-format codes &&& adds some features
</commit_message>
<xml_diff>
--- a/src/dataLocater/ExcelRead.xlsx
+++ b/src/dataLocater/ExcelRead.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="createAccuont" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="manufactureOrder" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="salesOrder" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t xml:space="preserve">testing</t>
   </si>
@@ -105,6 +106,30 @@
   </si>
   <si>
     <t xml:space="preserve">2020-03-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shipment Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ordered product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEFAS SILK PAINTS FACTORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addis Ababa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
   </si>
 </sst>
 </file>
@@ -115,7 +140,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -192,6 +217,17 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -248,7 +284,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -290,6 +326,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -579,7 +623,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -627,4 +671,76 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>